<commit_message>
LIVEHTA-2969 prod bug tc
</commit_message>
<xml_diff>
--- a/Testdata/PICOSPage_Data_Testing.xlsx
+++ b/Testdata/PICOSPage_Data_Testing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52479855-73A3-4775-A847-1CC1FF3179B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859E12D6-F0CE-4DB1-9952-C444A05A29D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>Economic</t>
   </si>
@@ -92,6 +92,45 @@
   </si>
   <si>
     <t>Exclusion Criteria</t>
+  </si>
+  <si>
+    <t>Population_Radio_button</t>
+  </si>
+  <si>
+    <t>slrtype</t>
+  </si>
+  <si>
+    <t>slrtype_Radio_button</t>
+  </si>
+  <si>
+    <t>Clinical_radio_button</t>
+  </si>
+  <si>
+    <t>Economic_radio_button</t>
+  </si>
+  <si>
+    <t>Quality of Life</t>
+  </si>
+  <si>
+    <t>Quality of Life_radio_button</t>
+  </si>
+  <si>
+    <t>Real-world Evidence_radio_button</t>
+  </si>
+  <si>
+    <t>Test_Sachin_2022 - Test_Sachin_radio_button</t>
+  </si>
+  <si>
+    <t>Adult patients (18 years or older) with maintenance therapy for NDMM after induction therapy, post-SCT*</t>
+  </si>
+  <si>
+    <t>Patients who do not undergo maintenance therapy
+Patients in later lines of therapy (not first line)
+Pediatric population
+Other types of cancers</t>
+  </si>
+  <si>
+    <t>data</t>
   </si>
 </sst>
 </file>
@@ -133,10 +172,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -418,39 +460,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -458,59 +513,95 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>17</v>
       </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>18</v>
       </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>13</v>
       </c>
+      <c r="G5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>